<commit_message>
fix export excel 2
</commit_message>
<xml_diff>
--- a/excelSheet/nhóm L1.xlsx
+++ b/excelSheet/nhóm L1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,95 +436,105 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>fullName</t>
+          <t>employeeId</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>level</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>teamName</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Loại</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>krId</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>KR phòng</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>KR team</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>KR cá nhân</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Công thức tính</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Nguồn dữ liệu</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Định kỳ tính</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Đơn vị tính</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Điều kiện</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Norm</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>% Trọng số chỉ tiêu</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Kết quả</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Tỷ lệ</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -532,93 +542,95 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B2" t="inlineStr">
+        <v>12</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>PHG</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>python</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>KPI</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>tét2321</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>tét2321</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>tét2321</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Báo cáo được CBQL confirm</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>MO</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>NUM</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>EQUAL</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
+          <t>Tháng</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
         <v>100</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>78</v>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>No data</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>No data</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr">
         <is>
           <t>168</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>168</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>dfqwq</t>
         </is>

</xml_diff>

<commit_message>
finish export kpi file
</commit_message>
<xml_diff>
--- a/excelSheet/nhóm L1.xlsx
+++ b/excelSheet/nhóm L1.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,15 +26,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF99"/>
+        <bgColor rgb="00FFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8CCE4"/>
+        <bgColor rgb="00B8CCE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00365072"/>
+        <bgColor rgb="00365072"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -46,19 +82,42 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,218 +484,283 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>employeeId</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>teamName</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Loại</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>krId</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>KR phòng</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>KR team</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>KR cá nhân</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Công thức tính</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Nguồn dữ liệu</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Định kỳ tính</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Đơn vị tính</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Điều kiện</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Norm</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>% Trọng số chỉ tiêu</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Kết quả</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Tỷ lệ</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nhóm L1</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>PHG</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>python</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Loại</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>KR phòng</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>KR team</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>KR cá nhân</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Công thức tính</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>Nguồn dữ liệu</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>Định kỳ tính</t>
+        </is>
+      </c>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>Đơn vị tính</t>
+        </is>
+      </c>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <t>Điều kiện</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="inlineStr">
+        <is>
+          <t>Norm</t>
+        </is>
+      </c>
+      <c r="K3" s="4" t="inlineStr">
+        <is>
+          <t>% Trọng số chỉ tiêu</t>
+        </is>
+      </c>
+      <c r="L3" s="4" t="inlineStr">
+        <is>
+          <t>Kết quả</t>
+        </is>
+      </c>
+      <c r="M3" s="4" t="inlineStr">
+        <is>
+          <t>Tỷ lệ</t>
+        </is>
+      </c>
+      <c r="N3" s="4" t="inlineStr">
+        <is>
+          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
+        </is>
+      </c>
+      <c r="O3" s="4" t="inlineStr">
+        <is>
+          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
+        </is>
+      </c>
+      <c r="P3" s="4" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>KPI</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>tét2321</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="C4" s="5" t="inlineStr">
         <is>
           <t>tét2321</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="D4" s="5" t="inlineStr">
         <is>
           <t>tét2321</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="E4" s="5" t="inlineStr">
         <is>
           <t>Báo cáo được CBQL confirm</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="G4" s="5" t="inlineStr">
         <is>
           <t>Tháng</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="H4" s="5" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="I4" s="5" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="P2" t="n">
+      <c r="J4" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="K4" s="5" t="n">
         <v>78</v>
       </c>
-      <c r="R2" t="n">
+      <c r="L4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="n">
+      <c r="M4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>168</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>168</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="N4" s="5" t="n">
+        <v>168</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <v>168</v>
+      </c>
+      <c r="P4" s="5" t="inlineStr">
         <is>
           <t>dfqwq</t>
         </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v/>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>78</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>168</v>
+      </c>
+      <c r="O5" s="6" t="n">
+        <v>168</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>